<commit_message>
Added ALUController and ALUController_tb.
</commit_message>
<xml_diff>
--- a/Control Signals.xlsx
+++ b/Control Signals.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10988" windowHeight="9083" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10992" windowHeight="9084" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -355,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -395,6 +395,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -404,7 +407,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -724,40 +727,40 @@
   <dimension ref="A1:X36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.9296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.3984375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="29.88671875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="17" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.3984375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.265625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" style="3" customWidth="1"/>
     <col min="7" max="7" width="7" style="3" customWidth="1"/>
     <col min="8" max="8" width="7.33203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="7.46484375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.06640625" style="3"/>
-    <col min="11" max="11" width="5.796875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="6.1328125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="7.44140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="3"/>
+    <col min="11" max="11" width="5.77734375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="6.109375" style="3" customWidth="1"/>
     <col min="13" max="13" width="9.6640625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.06640625" style="3"/>
-    <col min="15" max="15" width="7.19921875" style="3" customWidth="1"/>
-    <col min="16" max="16" width="10.265625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="7.19921875" style="3" customWidth="1"/>
-    <col min="18" max="18" width="7.73046875" style="3" customWidth="1"/>
-    <col min="19" max="19" width="9.06640625" style="3"/>
-    <col min="20" max="20" width="14.19921875" style="3" customWidth="1"/>
-    <col min="21" max="21" width="9.06640625" style="3"/>
-    <col min="22" max="22" width="10.73046875" style="3" customWidth="1"/>
-    <col min="23" max="16384" width="9.06640625" style="3"/>
+    <col min="14" max="14" width="9.109375" style="3"/>
+    <col min="15" max="15" width="7.21875" style="3" customWidth="1"/>
+    <col min="16" max="16" width="10.21875" style="3" customWidth="1"/>
+    <col min="17" max="17" width="7.21875" style="3" customWidth="1"/>
+    <col min="18" max="18" width="7.77734375" style="3" customWidth="1"/>
+    <col min="19" max="19" width="9.109375" style="3"/>
+    <col min="20" max="20" width="14.21875" style="3" customWidth="1"/>
+    <col min="21" max="21" width="9.109375" style="3"/>
+    <col min="22" max="22" width="10.77734375" style="3" customWidth="1"/>
+    <col min="23" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -819,7 +822,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>18</v>
       </c>
@@ -839,7 +842,7 @@
       <c r="G2" s="6">
         <v>0</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="19">
         <v>0</v>
       </c>
       <c r="I2" s="6">
@@ -881,7 +884,7 @@
       <c r="W2" s="7"/>
       <c r="X2" s="7"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>21</v>
       </c>
@@ -901,7 +904,7 @@
       <c r="G3" s="9">
         <v>0</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="15">
         <v>12</v>
       </c>
       <c r="I3" s="9">
@@ -943,7 +946,7 @@
       <c r="W3" s="7"/>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>30</v>
       </c>
@@ -963,7 +966,7 @@
       <c r="G4" s="9">
         <v>0</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="15">
         <v>3</v>
       </c>
       <c r="I4" s="9">
@@ -1005,16 +1008,18 @@
       <c r="W4" s="7"/>
       <c r="X4" s="7"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="D5" s="5">
-        <v>100111</v>
+        <v>1011</v>
       </c>
       <c r="E5" s="9">
         <v>0</v>
@@ -1025,8 +1030,8 @@
       <c r="G5" s="9">
         <v>0</v>
       </c>
-      <c r="H5" s="9">
-        <v>6</v>
+      <c r="H5" s="15">
+        <v>21</v>
       </c>
       <c r="I5" s="9">
         <v>1</v>
@@ -1059,24 +1064,26 @@
         <v>0</v>
       </c>
       <c r="S5" s="9">
-        <v>1</v>
-      </c>
-      <c r="T5" s="9" t="s">
-        <v>19</v>
+        <v>0</v>
+      </c>
+      <c r="T5" s="9">
+        <v>1</v>
       </c>
       <c r="W5" s="7"/>
       <c r="X5" s="7"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B6" s="5">
         <v>0</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="D6" s="5">
-        <v>100101</v>
+        <v>1010</v>
       </c>
       <c r="E6" s="9">
         <v>0</v>
@@ -1087,8 +1094,8 @@
       <c r="G6" s="9">
         <v>0</v>
       </c>
-      <c r="H6" s="9">
-        <v>4</v>
+      <c r="H6" s="15">
+        <v>21</v>
       </c>
       <c r="I6" s="9">
         <v>1</v>
@@ -1121,44 +1128,44 @@
         <v>0</v>
       </c>
       <c r="S6" s="9">
-        <v>1</v>
-      </c>
-      <c r="T6" s="9" t="s">
-        <v>19</v>
+        <v>0</v>
+      </c>
+      <c r="T6" s="9">
+        <v>0</v>
       </c>
       <c r="W6" s="7"/>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A7" s="10" t="s">
-        <v>47</v>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>25</v>
       </c>
       <c r="B7" s="5">
         <v>0</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D7" s="5">
-        <v>10</v>
+        <v>11000</v>
       </c>
       <c r="E7" s="9">
         <v>0</v>
       </c>
       <c r="F7" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="9">
         <v>0</v>
       </c>
-      <c r="H7" s="9">
-        <v>9</v>
-      </c>
-      <c r="I7" s="9">
-        <v>1</v>
+      <c r="H7" s="15">
+        <v>2</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="J7" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="9">
         <v>0</v>
@@ -1175,14 +1182,14 @@
       <c r="O7" s="9">
         <v>0</v>
       </c>
-      <c r="P7" s="9">
-        <v>1</v>
+      <c r="P7" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="Q7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="R7" s="9">
-        <v>0</v>
+      <c r="R7" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="S7" s="9">
         <v>1</v>
@@ -1193,36 +1200,36 @@
       <c r="W7" s="7"/>
       <c r="X7" s="7"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A8" s="10" t="s">
-        <v>46</v>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="B8" s="5">
         <v>0</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D8" s="5">
-        <v>110</v>
+        <v>11001</v>
       </c>
       <c r="E8" s="9">
         <v>0</v>
       </c>
       <c r="F8" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="9">
         <v>0</v>
       </c>
-      <c r="H8" s="9">
-        <v>20</v>
-      </c>
-      <c r="I8" s="9">
-        <v>1</v>
+      <c r="H8" s="15">
+        <v>13</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="J8" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="9">
         <v>0</v>
@@ -1239,14 +1246,14 @@
       <c r="O8" s="9">
         <v>0</v>
       </c>
-      <c r="P8" s="9">
-        <v>1</v>
+      <c r="P8" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="Q8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="R8" s="9">
-        <v>0</v>
+      <c r="R8" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="S8" s="9">
         <v>1</v>
@@ -1257,18 +1264,16 @@
       <c r="W8" s="7"/>
       <c r="X8" s="7"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B9" s="5">
         <v>0</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>60</v>
-      </c>
+      <c r="C9" s="5"/>
       <c r="D9" s="5">
-        <v>0</v>
+        <v>100111</v>
       </c>
       <c r="E9" s="9">
         <v>0</v>
@@ -1279,8 +1284,8 @@
       <c r="G9" s="9">
         <v>0</v>
       </c>
-      <c r="H9" s="9">
-        <v>7</v>
+      <c r="H9" s="15">
+        <v>6</v>
       </c>
       <c r="I9" s="9">
         <v>1</v>
@@ -1321,82 +1326,80 @@
       <c r="W9" s="7"/>
       <c r="X9" s="7"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B10" s="5">
         <v>0</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="C10" s="5"/>
       <c r="D10" s="5">
-        <v>100</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6">
-        <v>1</v>
-      </c>
-      <c r="G10" s="6">
-        <v>0</v>
-      </c>
-      <c r="H10" s="6">
-        <v>17</v>
-      </c>
-      <c r="I10" s="6">
-        <v>1</v>
-      </c>
-      <c r="J10" s="6">
-        <v>0</v>
-      </c>
-      <c r="K10" s="6">
-        <v>0</v>
-      </c>
-      <c r="L10" s="6">
-        <v>0</v>
-      </c>
-      <c r="M10" s="6">
-        <v>0</v>
-      </c>
-      <c r="N10" s="6">
-        <v>0</v>
-      </c>
-      <c r="O10" s="6">
-        <v>0</v>
-      </c>
-      <c r="P10" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R10" s="6">
-        <v>0</v>
-      </c>
-      <c r="S10" s="6">
-        <v>1</v>
-      </c>
-      <c r="T10" s="6" t="s">
+        <v>100101</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0</v>
+      </c>
+      <c r="H10" s="15">
+        <v>4</v>
+      </c>
+      <c r="I10" s="9">
+        <v>1</v>
+      </c>
+      <c r="J10" s="9">
+        <v>0</v>
+      </c>
+      <c r="K10" s="9">
+        <v>0</v>
+      </c>
+      <c r="L10" s="9">
+        <v>0</v>
+      </c>
+      <c r="M10" s="9">
+        <v>0</v>
+      </c>
+      <c r="N10" s="9">
+        <v>0</v>
+      </c>
+      <c r="O10" s="9">
+        <v>0</v>
+      </c>
+      <c r="P10" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R10" s="9">
+        <v>0</v>
+      </c>
+      <c r="S10" s="9">
+        <v>1</v>
+      </c>
+      <c r="T10" s="9" t="s">
         <v>19</v>
       </c>
       <c r="W10" s="7"/>
       <c r="X10" s="7"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B11" s="5">
         <v>0</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D11" s="5">
-        <v>101010</v>
+        <v>10</v>
       </c>
       <c r="E11" s="9">
         <v>0</v>
@@ -1407,8 +1410,8 @@
       <c r="G11" s="9">
         <v>0</v>
       </c>
-      <c r="H11" s="9">
-        <v>14</v>
+      <c r="H11" s="15">
+        <v>9</v>
       </c>
       <c r="I11" s="9">
         <v>1</v>
@@ -1449,18 +1452,18 @@
       <c r="W11" s="7"/>
       <c r="X11" s="7"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B12" s="5">
         <v>0</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="5">
-        <v>101011</v>
+        <v>110</v>
       </c>
       <c r="E12" s="9">
         <v>0</v>
@@ -1471,8 +1474,8 @@
       <c r="G12" s="9">
         <v>0</v>
       </c>
-      <c r="H12" s="9">
-        <v>16</v>
+      <c r="H12" s="15">
+        <v>20</v>
       </c>
       <c r="I12" s="9">
         <v>1</v>
@@ -1513,9 +1516,9 @@
       <c r="W12" s="7"/>
       <c r="X12" s="7"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B13" s="5">
         <v>0</v>
@@ -1524,7 +1527,7 @@
         <v>60</v>
       </c>
       <c r="D13" s="5">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E13" s="9">
         <v>0</v>
@@ -1535,8 +1538,8 @@
       <c r="G13" s="9">
         <v>0</v>
       </c>
-      <c r="H13" s="9">
-        <v>10</v>
+      <c r="H13" s="15">
+        <v>7</v>
       </c>
       <c r="I13" s="9">
         <v>1</v>
@@ -1577,9 +1580,9 @@
       <c r="W13" s="7"/>
       <c r="X13" s="7"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B14" s="5">
         <v>0</v>
@@ -1588,71 +1591,71 @@
         <v>58</v>
       </c>
       <c r="D14" s="5">
-        <v>111</v>
-      </c>
-      <c r="E14" s="9">
-        <v>0</v>
-      </c>
-      <c r="F14" s="9">
-        <v>1</v>
-      </c>
-      <c r="G14" s="9">
-        <v>0</v>
-      </c>
-      <c r="H14" s="9">
-        <v>19</v>
-      </c>
-      <c r="I14" s="9">
-        <v>1</v>
-      </c>
-      <c r="J14" s="9">
-        <v>0</v>
-      </c>
-      <c r="K14" s="9">
-        <v>0</v>
-      </c>
-      <c r="L14" s="9">
-        <v>0</v>
-      </c>
-      <c r="M14" s="9">
-        <v>0</v>
-      </c>
-      <c r="N14" s="9">
-        <v>0</v>
-      </c>
-      <c r="O14" s="9">
-        <v>0</v>
-      </c>
-      <c r="P14" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="R14" s="9">
-        <v>0</v>
-      </c>
-      <c r="S14" s="9">
-        <v>1</v>
-      </c>
-      <c r="T14" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
+      <c r="H14" s="19">
+        <v>17</v>
+      </c>
+      <c r="I14" s="6">
+        <v>1</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0</v>
+      </c>
+      <c r="L14" s="6">
+        <v>0</v>
+      </c>
+      <c r="M14" s="6">
+        <v>0</v>
+      </c>
+      <c r="N14" s="6">
+        <v>0</v>
+      </c>
+      <c r="O14" s="6">
+        <v>0</v>
+      </c>
+      <c r="P14" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R14" s="6">
+        <v>0</v>
+      </c>
+      <c r="S14" s="6">
+        <v>1</v>
+      </c>
+      <c r="T14" s="6" t="s">
         <v>19</v>
       </c>
       <c r="W14" s="7"/>
       <c r="X14" s="7"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B15" s="5">
         <v>0</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D15" s="5">
-        <v>10</v>
+        <v>101010</v>
       </c>
       <c r="E15" s="9">
         <v>0</v>
@@ -1663,8 +1666,8 @@
       <c r="G15" s="9">
         <v>0</v>
       </c>
-      <c r="H15" s="9">
-        <v>8</v>
+      <c r="H15" s="15">
+        <v>14</v>
       </c>
       <c r="I15" s="9">
         <v>1</v>
@@ -1705,18 +1708,18 @@
       <c r="W15" s="7"/>
       <c r="X15" s="7"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B16" s="5">
         <v>0</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D16" s="5">
-        <v>110</v>
+        <v>101011</v>
       </c>
       <c r="E16" s="9">
         <v>0</v>
@@ -1727,8 +1730,8 @@
       <c r="G16" s="9">
         <v>0</v>
       </c>
-      <c r="H16" s="9">
-        <v>18</v>
+      <c r="H16" s="15">
+        <v>16</v>
       </c>
       <c r="I16" s="9">
         <v>1</v>
@@ -1769,16 +1772,18 @@
       <c r="W16" s="7"/>
       <c r="X16" s="7"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A17" s="14" t="s">
-        <v>23</v>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="B17" s="5">
         <v>0</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="D17" s="5">
-        <v>100010</v>
+        <v>11</v>
       </c>
       <c r="E17" s="9">
         <v>0</v>
@@ -1789,8 +1794,8 @@
       <c r="G17" s="9">
         <v>0</v>
       </c>
-      <c r="H17" s="9">
-        <v>1</v>
+      <c r="H17" s="15">
+        <v>10</v>
       </c>
       <c r="I17" s="9">
         <v>1</v>
@@ -1831,16 +1836,18 @@
       <c r="W17" s="7"/>
       <c r="X17" s="7"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B18" s="5">
         <v>0</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="D18" s="5">
-        <v>100110</v>
+        <v>111</v>
       </c>
       <c r="E18" s="9">
         <v>0</v>
@@ -1851,8 +1858,8 @@
       <c r="G18" s="9">
         <v>0</v>
       </c>
-      <c r="H18" s="9">
-        <v>5</v>
+      <c r="H18" s="15">
+        <v>19</v>
       </c>
       <c r="I18" s="9">
         <v>1</v>
@@ -1893,18 +1900,18 @@
       <c r="W18" s="7"/>
       <c r="X18" s="7"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B19" s="5">
         <v>0</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D19" s="5">
-        <v>1011</v>
+        <v>10</v>
       </c>
       <c r="E19" s="9">
         <v>0</v>
@@ -1915,8 +1922,8 @@
       <c r="G19" s="9">
         <v>0</v>
       </c>
-      <c r="H19" s="9">
-        <v>21</v>
+      <c r="H19" s="15">
+        <v>8</v>
       </c>
       <c r="I19" s="9">
         <v>1</v>
@@ -1949,26 +1956,26 @@
         <v>0</v>
       </c>
       <c r="S19" s="9">
-        <v>0</v>
-      </c>
-      <c r="T19" s="9">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="T19" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="W19" s="7"/>
       <c r="X19" s="7"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B20" s="5">
         <v>0</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D20" s="5">
-        <v>1010</v>
+        <v>110</v>
       </c>
       <c r="E20" s="9">
         <v>0</v>
@@ -1979,8 +1986,8 @@
       <c r="G20" s="9">
         <v>0</v>
       </c>
-      <c r="H20" s="9">
-        <v>21</v>
+      <c r="H20" s="15">
+        <v>18</v>
       </c>
       <c r="I20" s="9">
         <v>1</v>
@@ -2013,44 +2020,42 @@
         <v>0</v>
       </c>
       <c r="S20" s="9">
-        <v>0</v>
-      </c>
-      <c r="T20" s="9">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="T20" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="W20" s="7"/>
       <c r="X20" s="7"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21" s="5">
         <v>0</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="C21" s="5"/>
       <c r="D21" s="5">
-        <v>11000</v>
+        <v>100010</v>
       </c>
       <c r="E21" s="9">
         <v>0</v>
       </c>
       <c r="F21" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="9">
         <v>0</v>
       </c>
-      <c r="H21" s="9">
-        <v>2</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>19</v>
+      <c r="H21" s="15">
+        <v>1</v>
+      </c>
+      <c r="I21" s="9">
+        <v>1</v>
       </c>
       <c r="J21" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" s="9">
         <v>0</v>
@@ -2067,14 +2072,14 @@
       <c r="O21" s="9">
         <v>0</v>
       </c>
-      <c r="P21" s="9" t="s">
-        <v>19</v>
+      <c r="P21" s="9">
+        <v>1</v>
       </c>
       <c r="Q21" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="R21" s="9" t="s">
-        <v>19</v>
+      <c r="R21" s="9">
+        <v>0</v>
       </c>
       <c r="S21" s="9">
         <v>1</v>
@@ -2085,36 +2090,34 @@
       <c r="W21" s="7"/>
       <c r="X21" s="7"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A22" s="14" t="s">
-        <v>26</v>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="B22" s="5">
         <v>0</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="C22" s="5"/>
       <c r="D22" s="5">
-        <v>11001</v>
+        <v>100110</v>
       </c>
       <c r="E22" s="9">
         <v>0</v>
       </c>
       <c r="F22" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="9">
         <v>0</v>
       </c>
-      <c r="H22" s="9">
-        <v>13</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>19</v>
+      <c r="H22" s="15">
+        <v>5</v>
+      </c>
+      <c r="I22" s="9">
+        <v>1</v>
       </c>
       <c r="J22" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" s="9">
         <v>0</v>
@@ -2131,14 +2134,14 @@
       <c r="O22" s="9">
         <v>0</v>
       </c>
-      <c r="P22" s="9" t="s">
-        <v>19</v>
+      <c r="P22" s="9">
+        <v>1</v>
       </c>
       <c r="Q22" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="R22" s="9" t="s">
-        <v>19</v>
+      <c r="R22" s="9">
+        <v>0</v>
       </c>
       <c r="S22" s="9">
         <v>1</v>
@@ -2149,7 +2152,7 @@
       <c r="W22" s="7"/>
       <c r="X22" s="7"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
         <v>22</v>
       </c>
@@ -2158,58 +2161,58 @@
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="18">
-        <v>0</v>
-      </c>
-      <c r="F23" s="18">
-        <v>1</v>
-      </c>
-      <c r="G23" s="18">
-        <v>1</v>
-      </c>
-      <c r="H23" s="18">
-        <v>0</v>
-      </c>
-      <c r="I23" s="18">
-        <v>0</v>
-      </c>
-      <c r="J23" s="18">
-        <v>0</v>
-      </c>
-      <c r="K23" s="18">
-        <v>0</v>
-      </c>
-      <c r="L23" s="18">
-        <v>0</v>
-      </c>
-      <c r="M23" s="18">
-        <v>0</v>
-      </c>
-      <c r="N23" s="18">
-        <v>0</v>
-      </c>
-      <c r="O23" s="18">
-        <v>0</v>
-      </c>
-      <c r="P23" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="R23" s="18">
-        <v>0</v>
-      </c>
-      <c r="S23" s="18">
-        <v>1</v>
-      </c>
-      <c r="T23" s="18" t="s">
+      <c r="E23" s="15">
+        <v>0</v>
+      </c>
+      <c r="F23" s="15">
+        <v>1</v>
+      </c>
+      <c r="G23" s="15">
+        <v>1</v>
+      </c>
+      <c r="H23" s="15">
+        <v>0</v>
+      </c>
+      <c r="I23" s="15">
+        <v>0</v>
+      </c>
+      <c r="J23" s="15">
+        <v>0</v>
+      </c>
+      <c r="K23" s="15">
+        <v>0</v>
+      </c>
+      <c r="L23" s="15">
+        <v>0</v>
+      </c>
+      <c r="M23" s="15">
+        <v>0</v>
+      </c>
+      <c r="N23" s="15">
+        <v>0</v>
+      </c>
+      <c r="O23" s="15">
+        <v>0</v>
+      </c>
+      <c r="P23" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="R23" s="15">
+        <v>0</v>
+      </c>
+      <c r="S23" s="15">
+        <v>1</v>
+      </c>
+      <c r="T23" s="15" t="s">
         <v>19</v>
       </c>
       <c r="W23" s="7"/>
       <c r="X23" s="7"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
         <v>20</v>
       </c>
@@ -2227,7 +2230,7 @@
       <c r="G24" s="9">
         <v>1</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="15">
         <v>12</v>
       </c>
       <c r="I24" s="9">
@@ -2269,7 +2272,7 @@
       <c r="W24" s="7"/>
       <c r="X24" s="7"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>43</v>
       </c>
@@ -2287,7 +2290,7 @@
       <c r="G25" s="9">
         <v>1</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="15">
         <v>14</v>
       </c>
       <c r="I25" s="9">
@@ -2329,7 +2332,7 @@
       <c r="W25" s="7"/>
       <c r="X25" s="7"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>51</v>
       </c>
@@ -2347,7 +2350,7 @@
       <c r="G26" s="9">
         <v>1</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H26" s="15">
         <v>16</v>
       </c>
       <c r="I26" s="9">
@@ -2387,7 +2390,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>31</v>
       </c>
@@ -2405,7 +2408,7 @@
       <c r="G27" s="9">
         <v>1</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="15">
         <v>3</v>
       </c>
       <c r="I27" s="9">
@@ -2445,7 +2448,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>35</v>
       </c>
@@ -2463,7 +2466,7 @@
       <c r="G28" s="9">
         <v>1</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="15">
         <v>4</v>
       </c>
       <c r="I28" s="9">
@@ -2503,7 +2506,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>36</v>
       </c>
@@ -2521,7 +2524,7 @@
       <c r="G29" s="9">
         <v>1</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="15">
         <v>5</v>
       </c>
       <c r="I29" s="9">
@@ -2561,39 +2564,39 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B30" s="5">
         <v>11100</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D30" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E30" s="9">
         <v>0</v>
       </c>
       <c r="F30" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30" s="9">
         <v>0</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="15">
         <v>2</v>
       </c>
-      <c r="I30" s="9">
-        <v>1</v>
+      <c r="I30" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="J30" s="9">
         <v>0</v>
       </c>
       <c r="K30" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" s="9">
         <v>0</v>
@@ -2607,14 +2610,14 @@
       <c r="O30" s="9">
         <v>0</v>
       </c>
-      <c r="P30" s="9">
-        <v>1</v>
+      <c r="P30" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="Q30" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="R30" s="9">
-        <v>0</v>
+      <c r="R30" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="S30" s="9">
         <v>1</v>
@@ -2623,9 +2626,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B31" s="5">
         <v>11100</v>
@@ -2634,7 +2637,7 @@
         <v>59</v>
       </c>
       <c r="D31" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E31" s="9">
         <v>0</v>
@@ -2645,7 +2648,7 @@
       <c r="G31" s="9">
         <v>0</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H31" s="15">
         <v>2</v>
       </c>
       <c r="I31" s="9" t="s">
@@ -2655,10 +2658,10 @@
         <v>0</v>
       </c>
       <c r="K31" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L31" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M31" s="9">
         <v>0</v>
@@ -2685,33 +2688,33 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B32" s="5">
         <v>11100</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D32" s="5">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="E32" s="9">
         <v>0</v>
       </c>
       <c r="F32" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32" s="9">
         <v>0</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H32" s="15">
         <v>2</v>
       </c>
-      <c r="I32" s="9" t="s">
-        <v>19</v>
+      <c r="I32" s="9">
+        <v>1</v>
       </c>
       <c r="J32" s="9">
         <v>0</v>
@@ -2720,7 +2723,7 @@
         <v>0</v>
       </c>
       <c r="L32" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32" s="9">
         <v>0</v>
@@ -2731,14 +2734,14 @@
       <c r="O32" s="9">
         <v>0</v>
       </c>
-      <c r="P32" s="9" t="s">
-        <v>19</v>
+      <c r="P32" s="9">
+        <v>1</v>
       </c>
       <c r="Q32" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="R32" s="9" t="s">
-        <v>19</v>
+      <c r="R32" s="9">
+        <v>0</v>
       </c>
       <c r="S32" s="9">
         <v>1</v>
@@ -2747,7 +2750,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>50</v>
       </c>
@@ -2769,7 +2772,7 @@
       <c r="G33" s="9">
         <v>0</v>
       </c>
-      <c r="H33" s="9">
+      <c r="H33" s="15">
         <v>15</v>
       </c>
       <c r="I33" s="9">
@@ -2809,7 +2812,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>37</v>
       </c>
@@ -2831,7 +2834,7 @@
       <c r="G34" s="9">
         <v>0</v>
       </c>
-      <c r="H34" s="9">
+      <c r="H34" s="15">
         <v>11</v>
       </c>
       <c r="I34" s="9">
@@ -2871,127 +2874,126 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="F35" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G35" s="15" t="s">
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H35" s="15" t="s">
+      <c r="H35" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I35" s="15" t="s">
+      <c r="I35" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J35" s="15" t="s">
+      <c r="J35" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="K35" s="15" t="s">
+      <c r="K35" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="L35" s="15" t="s">
+      <c r="L35" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="M35" s="15" t="s">
+      <c r="M35" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="N35" s="15" t="s">
+      <c r="N35" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="O35" s="15" t="s">
+      <c r="O35" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="P35" s="15" t="s">
+      <c r="P35" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="Q35" s="15" t="s">
+      <c r="Q35" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="R35" s="15" t="s">
+      <c r="R35" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="S35" s="15" t="s">
+      <c r="S35" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="T35" s="15" t="s">
+      <c r="T35" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G36" s="17" t="s">
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G36" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H36" s="17" t="s">
+      <c r="H36" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I36" s="17" t="s">
+      <c r="I36" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="J36" s="17" t="s">
+      <c r="J36" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="K36" s="17" t="s">
+      <c r="K36" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="L36" s="17" t="s">
+      <c r="L36" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="M36" s="17" t="s">
+      <c r="M36" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="N36" s="17" t="s">
+      <c r="N36" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="O36" s="17" t="s">
+      <c r="O36" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="P36" s="17" t="s">
+      <c r="P36" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="Q36" s="17" t="s">
+      <c r="Q36" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="R36" s="17" t="s">
+      <c r="R36" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="S36" s="17" t="s">
+      <c r="S36" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="T36" s="17" t="s">
+      <c r="T36" s="18" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:T36">
     <sortCondition ref="B2:B36"/>
-    <sortCondition descending="1" ref="F2:F36"/>
-    <sortCondition descending="1" ref="S2:S36"/>
+    <sortCondition ref="A2:A36"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Bug fixes... Now mthi, mtlo, mfhi, mflo all work with the given test cases now.
</commit_message>
<xml_diff>
--- a/Control Signals.xlsx
+++ b/Control Signals.xlsx
@@ -751,10 +751,10 @@
   <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T37" sqref="T37"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2957,7 +2957,9 @@
       <c r="G34" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H34" s="11"/>
+      <c r="H34" s="11">
+        <v>21</v>
+      </c>
       <c r="I34" s="10" t="s">
         <v>19</v>
       </c>
@@ -3020,7 +3022,9 @@
       <c r="G35" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H35" s="11"/>
+      <c r="H35" s="11">
+        <v>21</v>
+      </c>
       <c r="I35" s="10" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Fixed lb and lh. Now everything is working besides jumps
</commit_message>
<xml_diff>
--- a/Control Signals.xlsx
+++ b/Control Signals.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10990" windowHeight="3520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10988" windowHeight="3518" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="90">
   <si>
     <t>PCSrc</t>
   </si>
@@ -292,6 +292,12 @@
   </si>
   <si>
     <t>[20-16] = 00000</t>
+  </si>
+  <si>
+    <t>LoadExtended</t>
+  </si>
+  <si>
+    <t>Lb</t>
   </si>
 </sst>
 </file>
@@ -374,7 +380,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -447,11 +453,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -521,10 +538,19 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -844,40 +870,40 @@
   <dimension ref="A1:Y54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C40" sqref="C40"/>
+      <selection pane="bottomRight" activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1796875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.9296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.46484375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.59765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.46484375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.59765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.19921875" style="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.36328125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="7.453125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.08984375" style="1"/>
-    <col min="12" max="12" width="5.81640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.08984375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6328125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.08984375" style="1"/>
-    <col min="16" max="16" width="7.1796875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1796875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="7.1796875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="7.81640625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="9.08984375" style="1"/>
-    <col min="21" max="21" width="14.1796875" style="1" customWidth="1"/>
-    <col min="22" max="22" width="9.08984375" style="1"/>
-    <col min="23" max="23" width="10.81640625" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.08984375" style="1"/>
+    <col min="8" max="8" width="7.33203125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="7.46484375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.06640625" style="1"/>
+    <col min="12" max="12" width="5.796875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.06640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.59765625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.06640625" style="1"/>
+    <col min="16" max="16" width="7.19921875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="10.19921875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="7.19921875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="7.796875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="9.06640625" style="1"/>
+    <col min="21" max="21" width="14.19921875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="9.06640625" style="1"/>
+    <col min="23" max="23" width="13.6640625" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -941,8 +967,14 @@
       <c r="U1" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="V1" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="W1" s="26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A2" s="21" t="s">
         <v>16</v>
       </c>
@@ -962,7 +994,7 @@
       <c r="G2" s="7">
         <v>0</v>
       </c>
-      <c r="H2" s="25">
+      <c r="H2" s="8">
         <v>0</v>
       </c>
       <c r="I2" s="7">
@@ -1003,11 +1035,17 @@
       </c>
       <c r="U2" s="7" t="s">
         <v>17</v>
+      </c>
+      <c r="V2" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="W2" s="29">
+        <v>0</v>
       </c>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A3" s="23" t="s">
         <v>20</v>
       </c>
@@ -1025,7 +1063,7 @@
       <c r="G3" s="10">
         <v>1</v>
       </c>
-      <c r="H3" s="26">
+      <c r="H3" s="10">
         <v>0</v>
       </c>
       <c r="I3" s="10">
@@ -1066,11 +1104,17 @@
       </c>
       <c r="U3" s="10" t="s">
         <v>17</v>
+      </c>
+      <c r="V3" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="W3" s="29">
+        <v>0</v>
       </c>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>74</v>
       </c>
@@ -1088,7 +1132,7 @@
       <c r="G4" s="8">
         <v>1</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="8">
         <v>0</v>
       </c>
       <c r="I4" s="8">
@@ -1129,11 +1173,17 @@
       </c>
       <c r="U4" s="8" t="s">
         <v>17</v>
+      </c>
+      <c r="V4" s="27">
+        <v>1</v>
+      </c>
+      <c r="W4" s="8">
+        <v>1</v>
       </c>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>75</v>
       </c>
@@ -1151,7 +1201,7 @@
       <c r="G5" s="8">
         <v>1</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="8">
         <v>0</v>
       </c>
       <c r="I5" s="8">
@@ -1192,11 +1242,17 @@
       </c>
       <c r="U5" s="8" t="s">
         <v>17</v>
+      </c>
+      <c r="V5" s="28">
+        <v>0</v>
+      </c>
+      <c r="W5" s="8">
+        <v>1</v>
       </c>
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>70</v>
       </c>
@@ -1214,7 +1270,7 @@
       <c r="G6" s="8">
         <v>1</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="8">
         <v>0</v>
       </c>
       <c r="I6" s="8">
@@ -1255,11 +1311,17 @@
       </c>
       <c r="U6" s="8" t="s">
         <v>17</v>
+      </c>
+      <c r="V6" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="W6" s="29">
+        <v>0</v>
       </c>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>72</v>
       </c>
@@ -1275,7 +1337,7 @@
       <c r="G7" s="8">
         <v>1</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="8">
         <v>0</v>
       </c>
       <c r="I7" s="8" t="s">
@@ -1315,12 +1377,18 @@
         <v>17</v>
       </c>
       <c r="U7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="V7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W7" s="8" t="s">
         <v>17</v>
       </c>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>73</v>
       </c>
@@ -1336,7 +1404,7 @@
       <c r="G8" s="8">
         <v>1</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="8">
         <v>0</v>
       </c>
       <c r="I8" s="8" t="s">
@@ -1376,12 +1444,18 @@
         <v>17</v>
       </c>
       <c r="U8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="V8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W8" s="8" t="s">
         <v>17</v>
       </c>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>71</v>
       </c>
@@ -1399,7 +1473,7 @@
       <c r="G9" s="8">
         <v>1</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="8">
         <v>0</v>
       </c>
       <c r="I9" s="8" t="s">
@@ -1439,12 +1513,18 @@
         <v>17</v>
       </c>
       <c r="U9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="V9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W9" s="8" t="s">
         <v>17</v>
       </c>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A10" s="12" t="s">
         <v>21</v>
       </c>
@@ -1464,7 +1544,7 @@
       <c r="G10" s="9">
         <v>0</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="10">
         <v>1</v>
       </c>
       <c r="I10" s="9">
@@ -1505,11 +1585,17 @@
       </c>
       <c r="U10" s="9" t="s">
         <v>17</v>
+      </c>
+      <c r="V10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W10" s="29">
+        <v>0</v>
       </c>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A11" s="17" t="s">
         <v>78</v>
       </c>
@@ -1527,7 +1613,7 @@
       <c r="G11" s="14">
         <v>0</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="25">
         <v>1</v>
       </c>
       <c r="I11" s="14" t="s">
@@ -1567,12 +1653,18 @@
         <v>17</v>
       </c>
       <c r="U11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="V11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W11" s="27" t="s">
         <v>17</v>
       </c>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A12" s="24" t="s">
         <v>79</v>
       </c>
@@ -1590,7 +1682,7 @@
       <c r="G12" s="14">
         <v>0</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="25">
         <v>1</v>
       </c>
       <c r="I12" s="14" t="s">
@@ -1630,12 +1722,18 @@
         <v>17</v>
       </c>
       <c r="U12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="V12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W12" s="27" t="s">
         <v>17</v>
       </c>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A13" s="22" t="s">
         <v>23</v>
       </c>
@@ -1657,7 +1755,7 @@
       <c r="G13" s="9">
         <v>0</v>
       </c>
-      <c r="H13" s="26">
+      <c r="H13" s="10">
         <v>2</v>
       </c>
       <c r="I13" s="9" t="s">
@@ -1697,12 +1795,18 @@
         <v>1</v>
       </c>
       <c r="U13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="V13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W13" s="27" t="s">
         <v>17</v>
       </c>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A14" s="23" t="s">
         <v>25</v>
       </c>
@@ -1724,7 +1828,7 @@
       <c r="G14" s="9">
         <v>0</v>
       </c>
-      <c r="H14" s="26">
+      <c r="H14" s="10">
         <v>2</v>
       </c>
       <c r="I14" s="9" t="s">
@@ -1764,12 +1868,18 @@
         <v>1</v>
       </c>
       <c r="U14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="V14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W14" s="27" t="s">
         <v>17</v>
       </c>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A15" s="12" t="s">
         <v>26</v>
       </c>
@@ -1791,7 +1901,7 @@
       <c r="G15" s="9">
         <v>0</v>
       </c>
-      <c r="H15" s="26">
+      <c r="H15" s="10">
         <v>2</v>
       </c>
       <c r="I15" s="9" t="s">
@@ -1831,12 +1941,18 @@
         <v>1</v>
       </c>
       <c r="U15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="V15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W15" s="27" t="s">
         <v>17</v>
       </c>
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
@@ -1858,7 +1974,7 @@
       <c r="G16" s="9">
         <v>0</v>
       </c>
-      <c r="H16" s="26">
+      <c r="H16" s="10">
         <v>2</v>
       </c>
       <c r="I16" s="9">
@@ -1899,11 +2015,17 @@
       </c>
       <c r="U16" s="9" t="s">
         <v>17</v>
+      </c>
+      <c r="V16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W16" s="29">
+        <v>0</v>
       </c>
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>27</v>
       </c>
@@ -1923,7 +2045,7 @@
       <c r="G17" s="9">
         <v>0</v>
       </c>
-      <c r="H17" s="26">
+      <c r="H17" s="10">
         <v>3</v>
       </c>
       <c r="I17" s="9">
@@ -1964,11 +2086,17 @@
       </c>
       <c r="U17" s="9" t="s">
         <v>17</v>
+      </c>
+      <c r="V17" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W17" s="29">
+        <v>0</v>
       </c>
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>28</v>
       </c>
@@ -1986,7 +2114,7 @@
       <c r="G18" s="9">
         <v>1</v>
       </c>
-      <c r="H18" s="26">
+      <c r="H18" s="10">
         <v>3</v>
       </c>
       <c r="I18" s="9">
@@ -2027,11 +2155,17 @@
       </c>
       <c r="U18" s="9" t="s">
         <v>17</v>
+      </c>
+      <c r="V18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W18" s="29">
+        <v>0</v>
       </c>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
         <v>29</v>
       </c>
@@ -2051,7 +2185,7 @@
       <c r="G19" s="9">
         <v>0</v>
       </c>
-      <c r="H19" s="26">
+      <c r="H19" s="10">
         <v>4</v>
       </c>
       <c r="I19" s="9">
@@ -2092,11 +2226,17 @@
       </c>
       <c r="U19" s="9" t="s">
         <v>17</v>
+      </c>
+      <c r="V19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W19" s="29">
+        <v>0</v>
       </c>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
         <v>32</v>
       </c>
@@ -2114,7 +2254,7 @@
       <c r="G20" s="9">
         <v>1</v>
       </c>
-      <c r="H20" s="26">
+      <c r="H20" s="10">
         <v>4</v>
       </c>
       <c r="I20" s="9">
@@ -2155,11 +2295,17 @@
       </c>
       <c r="U20" s="9" t="s">
         <v>17</v>
+      </c>
+      <c r="V20" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W20" s="29">
+        <v>0</v>
       </c>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A21" s="11" t="s">
         <v>31</v>
       </c>
@@ -2179,7 +2325,7 @@
       <c r="G21" s="9">
         <v>0</v>
       </c>
-      <c r="H21" s="26">
+      <c r="H21" s="10">
         <v>5</v>
       </c>
       <c r="I21" s="9">
@@ -2220,11 +2366,17 @@
       </c>
       <c r="U21" s="9" t="s">
         <v>17</v>
+      </c>
+      <c r="V21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W21" s="29">
+        <v>0</v>
       </c>
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A22" s="11" t="s">
         <v>33</v>
       </c>
@@ -2242,7 +2394,7 @@
       <c r="G22" s="9">
         <v>1</v>
       </c>
-      <c r="H22" s="26">
+      <c r="H22" s="10">
         <v>5</v>
       </c>
       <c r="I22" s="9">
@@ -2283,11 +2435,17 @@
       </c>
       <c r="U22" s="9" t="s">
         <v>17</v>
+      </c>
+      <c r="V22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W22" s="29">
+        <v>0</v>
       </c>
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
         <v>30</v>
       </c>
@@ -2307,7 +2465,7 @@
       <c r="G23" s="9">
         <v>0</v>
       </c>
-      <c r="H23" s="26">
+      <c r="H23" s="10">
         <v>6</v>
       </c>
       <c r="I23" s="9">
@@ -2348,11 +2506,17 @@
       </c>
       <c r="U23" s="9" t="s">
         <v>17</v>
+      </c>
+      <c r="V23" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W23" s="29">
+        <v>0</v>
       </c>
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A24" s="11" t="s">
         <v>35</v>
       </c>
@@ -2374,7 +2538,7 @@
       <c r="G24" s="9">
         <v>0</v>
       </c>
-      <c r="H24" s="26">
+      <c r="H24" s="10">
         <v>7</v>
       </c>
       <c r="I24" s="9">
@@ -2415,11 +2579,17 @@
       </c>
       <c r="U24" s="9" t="s">
         <v>17</v>
+      </c>
+      <c r="V24" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W24" s="29">
+        <v>0</v>
       </c>
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A25" s="11" t="s">
         <v>36</v>
       </c>
@@ -2441,7 +2611,7 @@
       <c r="G25" s="9">
         <v>0</v>
       </c>
-      <c r="H25" s="26">
+      <c r="H25" s="10">
         <v>8</v>
       </c>
       <c r="I25" s="9">
@@ -2482,11 +2652,17 @@
       </c>
       <c r="U25" s="9" t="s">
         <v>17</v>
+      </c>
+      <c r="V25" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W25" s="29">
+        <v>0</v>
       </c>
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A26" s="11" t="s">
         <v>44</v>
       </c>
@@ -2508,7 +2684,7 @@
       <c r="G26" s="9">
         <v>0</v>
       </c>
-      <c r="H26" s="26">
+      <c r="H26" s="10">
         <v>9</v>
       </c>
       <c r="I26" s="9">
@@ -2550,8 +2726,14 @@
       <c r="U26" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="V26" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W26" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A27" s="11" t="s">
         <v>45</v>
       </c>
@@ -2573,7 +2755,7 @@
       <c r="G27" s="9">
         <v>0</v>
       </c>
-      <c r="H27" s="26">
+      <c r="H27" s="10">
         <v>10</v>
       </c>
       <c r="I27" s="9">
@@ -2615,8 +2797,14 @@
       <c r="U27" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="V27" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W27" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
         <v>34</v>
       </c>
@@ -2638,7 +2826,7 @@
       <c r="G28" s="9">
         <v>0</v>
       </c>
-      <c r="H28" s="26">
+      <c r="H28" s="10">
         <v>11</v>
       </c>
       <c r="I28" s="9">
@@ -2680,8 +2868,14 @@
       <c r="U28" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="V28" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W28" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A29" s="12" t="s">
         <v>19</v>
       </c>
@@ -2701,7 +2895,7 @@
       <c r="G29" s="9">
         <v>0</v>
       </c>
-      <c r="H29" s="26">
+      <c r="H29" s="10">
         <v>12</v>
       </c>
       <c r="I29" s="9">
@@ -2743,8 +2937,14 @@
       <c r="U29" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="V29" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W29" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A30" s="12" t="s">
         <v>18</v>
       </c>
@@ -2762,7 +2962,7 @@
       <c r="G30" s="9">
         <v>1</v>
       </c>
-      <c r="H30" s="26">
+      <c r="H30" s="10">
         <v>12</v>
       </c>
       <c r="I30" s="9">
@@ -2804,8 +3004,14 @@
       <c r="U30" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="V30" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W30" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A31" s="12" t="s">
         <v>24</v>
       </c>
@@ -2827,7 +3033,7 @@
       <c r="G31" s="9">
         <v>0</v>
       </c>
-      <c r="H31" s="26">
+      <c r="H31" s="10">
         <v>13</v>
       </c>
       <c r="I31" s="9" t="s">
@@ -2869,8 +3075,14 @@
       <c r="U31" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="V31" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W31" s="27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A32" s="11" t="s">
         <v>39</v>
       </c>
@@ -2892,7 +3104,7 @@
       <c r="G32" s="9">
         <v>0</v>
       </c>
-      <c r="H32" s="26">
+      <c r="H32" s="10">
         <v>14</v>
       </c>
       <c r="I32" s="9">
@@ -2934,8 +3146,14 @@
       <c r="U32" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V32" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W32" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A33" s="11" t="s">
         <v>40</v>
       </c>
@@ -2953,7 +3171,7 @@
       <c r="G33" s="9">
         <v>1</v>
       </c>
-      <c r="H33" s="26">
+      <c r="H33" s="10">
         <v>14</v>
       </c>
       <c r="I33" s="9">
@@ -2995,8 +3213,14 @@
       <c r="U33" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V33" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W33" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A34" s="11" t="s">
         <v>47</v>
       </c>
@@ -3018,7 +3242,7 @@
       <c r="G34" s="9">
         <v>0</v>
       </c>
-      <c r="H34" s="26">
+      <c r="H34" s="10">
         <v>15</v>
       </c>
       <c r="I34" s="9">
@@ -3060,8 +3284,14 @@
       <c r="U34" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V34" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W34" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A35" s="11" t="s">
         <v>49</v>
       </c>
@@ -3083,7 +3313,7 @@
       <c r="G35" s="9">
         <v>0</v>
       </c>
-      <c r="H35" s="26">
+      <c r="H35" s="10">
         <v>16</v>
       </c>
       <c r="I35" s="9">
@@ -3125,8 +3355,14 @@
       <c r="U35" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V35" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W35" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A36" s="11" t="s">
         <v>48</v>
       </c>
@@ -3144,7 +3380,7 @@
       <c r="G36" s="9">
         <v>1</v>
       </c>
-      <c r="H36" s="26">
+      <c r="H36" s="10">
         <v>16</v>
       </c>
       <c r="I36" s="9">
@@ -3186,8 +3422,14 @@
       <c r="U36" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V36" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W36" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A37" s="11" t="s">
         <v>37</v>
       </c>
@@ -3209,7 +3451,7 @@
       <c r="G37" s="7">
         <v>0</v>
       </c>
-      <c r="H37" s="25">
+      <c r="H37" s="8">
         <v>17</v>
       </c>
       <c r="I37" s="7">
@@ -3251,8 +3493,14 @@
       <c r="U37" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V37" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W37" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A38" s="11" t="s">
         <v>38</v>
       </c>
@@ -3274,7 +3522,7 @@
       <c r="G38" s="9">
         <v>0</v>
       </c>
-      <c r="H38" s="26">
+      <c r="H38" s="10">
         <v>18</v>
       </c>
       <c r="I38" s="9">
@@ -3316,8 +3564,14 @@
       <c r="U38" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V38" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W38" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A39" s="11" t="s">
         <v>46</v>
       </c>
@@ -3339,7 +3593,7 @@
       <c r="G39" s="9">
         <v>0</v>
       </c>
-      <c r="H39" s="26">
+      <c r="H39" s="10">
         <v>19</v>
       </c>
       <c r="I39" s="9">
@@ -3381,8 +3635,14 @@
       <c r="U39" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V39" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W39" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A40" s="11" t="s">
         <v>43</v>
       </c>
@@ -3404,7 +3664,7 @@
       <c r="G40" s="9">
         <v>0</v>
       </c>
-      <c r="H40" s="26">
+      <c r="H40" s="10">
         <v>20</v>
       </c>
       <c r="I40" s="9">
@@ -3446,8 +3706,14 @@
       <c r="U40" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V40" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W40" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A41" s="11" t="s">
         <v>41</v>
       </c>
@@ -3469,7 +3735,7 @@
       <c r="G41" s="9">
         <v>0</v>
       </c>
-      <c r="H41" s="26">
+      <c r="H41" s="10">
         <v>21</v>
       </c>
       <c r="I41" s="9">
@@ -3511,8 +3777,14 @@
       <c r="U41" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V41" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W41" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A42" s="11" t="s">
         <v>42</v>
       </c>
@@ -3534,7 +3806,7 @@
       <c r="G42" s="9">
         <v>0</v>
       </c>
-      <c r="H42" s="26">
+      <c r="H42" s="10">
         <v>21</v>
       </c>
       <c r="I42" s="9">
@@ -3576,8 +3848,14 @@
       <c r="U42" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V42" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W42" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>66</v>
       </c>
@@ -3599,7 +3877,7 @@
       <c r="G43" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H43" s="26">
+      <c r="H43" s="10">
         <v>21</v>
       </c>
       <c r="I43" s="9" t="s">
@@ -3641,8 +3919,14 @@
       <c r="U43" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V43" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W43" s="27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>64</v>
       </c>
@@ -3664,7 +3948,7 @@
       <c r="G44" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H44" s="26">
+      <c r="H44" s="10">
         <v>21</v>
       </c>
       <c r="I44" s="9" t="s">
@@ -3706,8 +3990,14 @@
       <c r="U44" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V44" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W44" s="27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A45" s="13" t="s">
         <v>76</v>
       </c>
@@ -3725,7 +4015,7 @@
       <c r="G45" s="15">
         <v>1</v>
       </c>
-      <c r="H45" s="19">
+      <c r="H45" s="25">
         <v>22</v>
       </c>
       <c r="I45" s="15">
@@ -3767,8 +4057,14 @@
       <c r="U45" s="14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V45" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W45" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A46" s="17" t="s">
         <v>82</v>
       </c>
@@ -3788,7 +4084,7 @@
       <c r="G46" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H46" s="19">
+      <c r="H46" s="25">
         <v>23</v>
       </c>
       <c r="I46" s="14" t="s">
@@ -3830,8 +4126,14 @@
       <c r="U46" s="14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V46" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W46" s="27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A47" s="17" t="s">
         <v>81</v>
       </c>
@@ -3851,7 +4153,7 @@
       <c r="G47" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H47" s="19">
+      <c r="H47" s="25">
         <v>24</v>
       </c>
       <c r="I47" s="14" t="s">
@@ -3893,8 +4195,14 @@
       <c r="U47" s="14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V47" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W47" s="27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A48" s="17" t="s">
         <v>80</v>
       </c>
@@ -3914,7 +4222,7 @@
       <c r="G48" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H48" s="19">
+      <c r="H48" s="25">
         <v>25</v>
       </c>
       <c r="I48" s="14" t="s">
@@ -3956,8 +4264,14 @@
       <c r="U48" s="14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V48" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W48" s="27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A49" s="17" t="s">
         <v>77</v>
       </c>
@@ -3977,7 +4291,7 @@
       <c r="G49" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H49" s="19">
+      <c r="H49" s="25">
         <v>26</v>
       </c>
       <c r="I49" s="14" t="s">
@@ -4019,8 +4333,14 @@
       <c r="U49" s="14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V49" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W49" s="27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
         <v>69</v>
       </c>
@@ -4042,7 +4362,7 @@
       <c r="G50" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H50" s="26" t="s">
+      <c r="H50" s="10" t="s">
         <v>17</v>
       </c>
       <c r="I50" s="9">
@@ -4084,8 +4404,14 @@
       <c r="U50" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V50" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W50" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A51" s="3" t="s">
         <v>67</v>
       </c>
@@ -4107,7 +4433,7 @@
       <c r="G51" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H51" s="26" t="s">
+      <c r="H51" s="10" t="s">
         <v>17</v>
       </c>
       <c r="I51" s="9">
@@ -4149,8 +4475,14 @@
       <c r="U51" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V51" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="W51" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A52" s="17" t="s">
         <v>84</v>
       </c>
@@ -4179,7 +4511,7 @@
       <c r="T52" s="15"/>
       <c r="U52" s="15"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A53" s="17" t="s">
         <v>83</v>
       </c>
@@ -4206,7 +4538,7 @@
       <c r="T53" s="15"/>
       <c r="U53" s="15"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A54" s="17" t="s">
         <v>85</v>
       </c>

</xml_diff>